<commit_message>
Merged code with one Integration Test
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/TestData/TestData.xlsx
+++ b/TGLAutomation/src/test/resources/TestData/TestData.xlsx
@@ -230,10 +230,10 @@
     <t>Login_PasswordOnline</t>
   </si>
   <si>
-    <t xml:space="preserve">kea54@georgetown.edu </t>
-  </si>
-  <si>
-    <t>4314574</t>
+    <t>4327757</t>
+  </si>
+  <si>
+    <t>yendeli98@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1039,13 +1039,13 @@
         <v>38</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Test case fixes - AppCenterIntegration Tests
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/TestData/TestData.xlsx
+++ b/TGLAutomation/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TGL\TGL_Branch\tgl-selenium-automation\TGLAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Local_Rep\TGLAdmin\tgl-selenium-automation\TGLAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE5EF1D-4B61-4ACD-8654-9EB8A751CBB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="TGLTestData" sheetId="8" r:id="rId1"/>
@@ -24,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nitin Sharma</author>
+  </authors>
+  <commentList>
+    <comment ref="F5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nitin Sharma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+change email id according to PIDIntegration value</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
@@ -228,17 +261,17 @@
     <t>Login_PasswordOnline</t>
   </si>
   <si>
-    <t>yendeli98@gmail.com</t>
-  </si>
-  <si>
     <t>4118889</t>
+  </si>
+  <si>
+    <t>meeyaaken2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +307,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -671,102 +717,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="40.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="33.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="33.44140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="38.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="38.140625" style="3" customWidth="1"/>
     <col min="16" max="16" width="34" style="3" customWidth="1"/>
-    <col min="17" max="17" width="34.88671875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="34.85546875" style="3" customWidth="1"/>
     <col min="18" max="18" width="35" style="3" customWidth="1"/>
-    <col min="19" max="19" width="31.5546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="35.44140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="25.44140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="34.5546875" style="3" customWidth="1"/>
-    <col min="23" max="23" width="34.44140625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="41.5546875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="40.109375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="41.6640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="40.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="43.6640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="33.5546875" style="3" customWidth="1"/>
-    <col min="30" max="30" width="43.44140625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="35.6640625" style="3" customWidth="1"/>
-    <col min="32" max="32" width="30.6640625" style="3" customWidth="1"/>
-    <col min="33" max="34" width="34.33203125" style="3" customWidth="1"/>
-    <col min="35" max="35" width="41.33203125" style="3" customWidth="1"/>
-    <col min="36" max="36" width="21.5546875" style="3" customWidth="1"/>
-    <col min="37" max="37" width="28.6640625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="25.88671875" style="3" customWidth="1"/>
-    <col min="39" max="39" width="28.33203125" style="3" customWidth="1"/>
-    <col min="40" max="40" width="27.33203125" style="3" customWidth="1"/>
-    <col min="41" max="41" width="23.6640625" style="3" customWidth="1"/>
-    <col min="42" max="42" width="29.88671875" style="3" customWidth="1"/>
-    <col min="43" max="43" width="25.5546875" style="3" customWidth="1"/>
-    <col min="44" max="45" width="29.109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="31.5703125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="34.5703125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="34.42578125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="41.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="40.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="41.7109375" style="3" customWidth="1"/>
+    <col min="27" max="27" width="40.42578125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="43.7109375" style="3" customWidth="1"/>
+    <col min="29" max="29" width="33.5703125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="43.42578125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="35.7109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="30.7109375" style="3" customWidth="1"/>
+    <col min="33" max="34" width="34.28515625" style="3" customWidth="1"/>
+    <col min="35" max="35" width="41.28515625" style="3" customWidth="1"/>
+    <col min="36" max="36" width="21.5703125" style="3" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" style="3" customWidth="1"/>
+    <col min="38" max="38" width="25.85546875" style="3" customWidth="1"/>
+    <col min="39" max="39" width="28.28515625" style="3" customWidth="1"/>
+    <col min="40" max="40" width="27.28515625" style="3" customWidth="1"/>
+    <col min="41" max="41" width="23.7109375" style="3" customWidth="1"/>
+    <col min="42" max="42" width="29.85546875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="25.5703125" style="3" customWidth="1"/>
+    <col min="44" max="45" width="29.140625" style="3" customWidth="1"/>
     <col min="46" max="46" width="30" style="3" customWidth="1"/>
-    <col min="47" max="47" width="23.6640625" style="3" customWidth="1"/>
-    <col min="48" max="49" width="26.109375" style="3" customWidth="1"/>
-    <col min="50" max="50" width="26.5546875" style="3" customWidth="1"/>
-    <col min="51" max="51" width="16.88671875" style="3" customWidth="1"/>
-    <col min="52" max="52" width="29.88671875" style="3" customWidth="1"/>
-    <col min="53" max="53" width="37.33203125" style="3" customWidth="1"/>
-    <col min="54" max="61" width="9.109375" style="3"/>
-    <col min="62" max="62" width="36.88671875" style="3" customWidth="1"/>
-    <col min="63" max="63" width="9.109375" style="3"/>
+    <col min="47" max="47" width="23.7109375" style="3" customWidth="1"/>
+    <col min="48" max="49" width="26.140625" style="3" customWidth="1"/>
+    <col min="50" max="50" width="26.5703125" style="3" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" style="3" customWidth="1"/>
+    <col min="52" max="52" width="29.85546875" style="3" customWidth="1"/>
+    <col min="53" max="53" width="37.28515625" style="3" customWidth="1"/>
+    <col min="54" max="61" width="9.140625" style="3"/>
+    <col min="62" max="62" width="36.85546875" style="3" customWidth="1"/>
+    <col min="63" max="63" width="9.140625" style="3"/>
     <col min="64" max="64" width="25" style="3" customWidth="1"/>
-    <col min="65" max="65" width="35.6640625" style="3" customWidth="1"/>
-    <col min="66" max="66" width="39.33203125" style="3" customWidth="1"/>
-    <col min="67" max="67" width="31.44140625" style="3" customWidth="1"/>
-    <col min="68" max="69" width="9.109375" style="3"/>
-    <col min="70" max="70" width="29.44140625" style="3" customWidth="1"/>
-    <col min="71" max="71" width="36.88671875" style="3" customWidth="1"/>
-    <col min="72" max="72" width="26.5546875" style="3" customWidth="1"/>
-    <col min="73" max="73" width="33.33203125" style="3" customWidth="1"/>
-    <col min="74" max="74" width="37.6640625" style="3" customWidth="1"/>
-    <col min="75" max="75" width="35.109375" style="3" customWidth="1"/>
-    <col min="76" max="76" width="36.5546875" style="3" customWidth="1"/>
-    <col min="77" max="77" width="19.88671875" style="3" customWidth="1"/>
-    <col min="78" max="78" width="31.5546875" style="3" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" style="3" customWidth="1"/>
-    <col min="80" max="80" width="21.88671875" style="3" customWidth="1"/>
-    <col min="81" max="81" width="20.6640625" style="3" customWidth="1"/>
-    <col min="82" max="82" width="38.88671875" style="3" customWidth="1"/>
-    <col min="83" max="83" width="25.44140625" style="3" customWidth="1"/>
-    <col min="84" max="84" width="33.5546875" style="3" customWidth="1"/>
-    <col min="85" max="85" width="35.33203125" style="3" customWidth="1"/>
-    <col min="86" max="86" width="35.6640625" style="3" customWidth="1"/>
-    <col min="87" max="87" width="32.33203125" style="3" customWidth="1"/>
-    <col min="88" max="88" width="29.6640625" style="3" customWidth="1"/>
-    <col min="89" max="89" width="19.6640625" style="3" customWidth="1"/>
-    <col min="90" max="90" width="24.44140625" style="3" customWidth="1"/>
-    <col min="91" max="91" width="32.44140625" style="3" customWidth="1"/>
-    <col min="92" max="92" width="36.88671875" style="3" customWidth="1"/>
-    <col min="93" max="93" width="14.5546875" style="3" customWidth="1"/>
-    <col min="94" max="16384" width="9.109375" style="3"/>
+    <col min="65" max="65" width="35.7109375" style="3" customWidth="1"/>
+    <col min="66" max="66" width="39.28515625" style="3" customWidth="1"/>
+    <col min="67" max="67" width="31.42578125" style="3" customWidth="1"/>
+    <col min="68" max="69" width="9.140625" style="3"/>
+    <col min="70" max="70" width="29.42578125" style="3" customWidth="1"/>
+    <col min="71" max="71" width="36.85546875" style="3" customWidth="1"/>
+    <col min="72" max="72" width="26.5703125" style="3" customWidth="1"/>
+    <col min="73" max="73" width="33.28515625" style="3" customWidth="1"/>
+    <col min="74" max="74" width="37.7109375" style="3" customWidth="1"/>
+    <col min="75" max="75" width="35.140625" style="3" customWidth="1"/>
+    <col min="76" max="76" width="36.5703125" style="3" customWidth="1"/>
+    <col min="77" max="77" width="19.85546875" style="3" customWidth="1"/>
+    <col min="78" max="78" width="31.5703125" style="3" customWidth="1"/>
+    <col min="79" max="79" width="19.28515625" style="3" customWidth="1"/>
+    <col min="80" max="80" width="21.85546875" style="3" customWidth="1"/>
+    <col min="81" max="81" width="20.7109375" style="3" customWidth="1"/>
+    <col min="82" max="82" width="38.85546875" style="3" customWidth="1"/>
+    <col min="83" max="83" width="25.42578125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="33.5703125" style="3" customWidth="1"/>
+    <col min="85" max="85" width="35.28515625" style="3" customWidth="1"/>
+    <col min="86" max="86" width="35.7109375" style="3" customWidth="1"/>
+    <col min="87" max="87" width="32.28515625" style="3" customWidth="1"/>
+    <col min="88" max="88" width="29.7109375" style="3" customWidth="1"/>
+    <col min="89" max="89" width="19.7109375" style="3" customWidth="1"/>
+    <col min="90" max="90" width="24.42578125" style="3" customWidth="1"/>
+    <col min="91" max="91" width="32.42578125" style="3" customWidth="1"/>
+    <col min="92" max="92" width="36.85546875" style="3" customWidth="1"/>
+    <col min="93" max="93" width="14.5703125" style="3" customWidth="1"/>
+    <col min="94" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -858,7 +904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -946,7 +992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1029,7 @@
       <c r="T3" s="6"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1066,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1037,22 +1083,22 @@
         <v>38</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="3">
-        <v>4327757</v>
+      <c r="H5" s="6">
+        <v>4373388</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -1067,11 +1113,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set up test data for integration test after qa fresh
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/TestData/TestData.xlsx
+++ b/TGLAutomation/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TGL\TGLNEW\tgl-selenium-automation\TGLAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Local_Rep\TGLAdmin\tgl-selenium-automation\TGLAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5597D1-14D7-4E71-BAD1-9DEEE1E7C334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="TGLTestData" sheetId="8" r:id="rId1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nitin Sharma</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>S.N.</t>
   </si>
@@ -262,16 +261,13 @@
     <t>Login_PasswordOnline</t>
   </si>
   <si>
-    <t>4118889</t>
-  </si>
-  <si>
-    <t>meeyaaken2@gmail.com</t>
+    <t>amadasun@usc.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -718,102 +714,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="40.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="37.44140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="33.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="33.44140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="38.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="40.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="33.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="38.140625" style="3" customWidth="1"/>
     <col min="16" max="16" width="34" style="3" customWidth="1"/>
-    <col min="17" max="17" width="34.88671875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="34.85546875" style="3" customWidth="1"/>
     <col min="18" max="18" width="35" style="3" customWidth="1"/>
-    <col min="19" max="19" width="31.5546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="35.44140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="25.44140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="34.5546875" style="3" customWidth="1"/>
-    <col min="23" max="23" width="34.44140625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="41.5546875" style="3" customWidth="1"/>
-    <col min="25" max="25" width="40.109375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="41.6640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="40.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="43.6640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="33.5546875" style="3" customWidth="1"/>
-    <col min="30" max="30" width="43.44140625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="35.6640625" style="3" customWidth="1"/>
-    <col min="32" max="32" width="30.6640625" style="3" customWidth="1"/>
-    <col min="33" max="34" width="34.33203125" style="3" customWidth="1"/>
-    <col min="35" max="35" width="41.33203125" style="3" customWidth="1"/>
-    <col min="36" max="36" width="21.5546875" style="3" customWidth="1"/>
-    <col min="37" max="37" width="28.6640625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="25.88671875" style="3" customWidth="1"/>
-    <col min="39" max="39" width="28.33203125" style="3" customWidth="1"/>
-    <col min="40" max="40" width="27.33203125" style="3" customWidth="1"/>
-    <col min="41" max="41" width="23.6640625" style="3" customWidth="1"/>
-    <col min="42" max="42" width="29.88671875" style="3" customWidth="1"/>
-    <col min="43" max="43" width="25.5546875" style="3" customWidth="1"/>
-    <col min="44" max="45" width="29.109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="31.5703125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="34.5703125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="34.42578125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="41.5703125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="40.140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="41.7109375" style="3" customWidth="1"/>
+    <col min="27" max="27" width="40.42578125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="43.7109375" style="3" customWidth="1"/>
+    <col min="29" max="29" width="33.5703125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="43.42578125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="35.7109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="30.7109375" style="3" customWidth="1"/>
+    <col min="33" max="34" width="34.28515625" style="3" customWidth="1"/>
+    <col min="35" max="35" width="41.28515625" style="3" customWidth="1"/>
+    <col min="36" max="36" width="21.5703125" style="3" customWidth="1"/>
+    <col min="37" max="37" width="28.7109375" style="3" customWidth="1"/>
+    <col min="38" max="38" width="25.85546875" style="3" customWidth="1"/>
+    <col min="39" max="39" width="28.28515625" style="3" customWidth="1"/>
+    <col min="40" max="40" width="27.28515625" style="3" customWidth="1"/>
+    <col min="41" max="41" width="23.7109375" style="3" customWidth="1"/>
+    <col min="42" max="42" width="29.85546875" style="3" customWidth="1"/>
+    <col min="43" max="43" width="25.5703125" style="3" customWidth="1"/>
+    <col min="44" max="45" width="29.140625" style="3" customWidth="1"/>
     <col min="46" max="46" width="30" style="3" customWidth="1"/>
-    <col min="47" max="47" width="23.6640625" style="3" customWidth="1"/>
-    <col min="48" max="49" width="26.109375" style="3" customWidth="1"/>
-    <col min="50" max="50" width="26.5546875" style="3" customWidth="1"/>
-    <col min="51" max="51" width="16.88671875" style="3" customWidth="1"/>
-    <col min="52" max="52" width="29.88671875" style="3" customWidth="1"/>
-    <col min="53" max="53" width="37.33203125" style="3" customWidth="1"/>
-    <col min="54" max="61" width="9.109375" style="3"/>
-    <col min="62" max="62" width="36.88671875" style="3" customWidth="1"/>
-    <col min="63" max="63" width="9.109375" style="3"/>
+    <col min="47" max="47" width="23.7109375" style="3" customWidth="1"/>
+    <col min="48" max="49" width="26.140625" style="3" customWidth="1"/>
+    <col min="50" max="50" width="26.5703125" style="3" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" style="3" customWidth="1"/>
+    <col min="52" max="52" width="29.85546875" style="3" customWidth="1"/>
+    <col min="53" max="53" width="37.28515625" style="3" customWidth="1"/>
+    <col min="54" max="61" width="9.140625" style="3"/>
+    <col min="62" max="62" width="36.85546875" style="3" customWidth="1"/>
+    <col min="63" max="63" width="9.140625" style="3"/>
     <col min="64" max="64" width="25" style="3" customWidth="1"/>
-    <col min="65" max="65" width="35.6640625" style="3" customWidth="1"/>
-    <col min="66" max="66" width="39.33203125" style="3" customWidth="1"/>
-    <col min="67" max="67" width="31.44140625" style="3" customWidth="1"/>
-    <col min="68" max="69" width="9.109375" style="3"/>
-    <col min="70" max="70" width="29.44140625" style="3" customWidth="1"/>
-    <col min="71" max="71" width="36.88671875" style="3" customWidth="1"/>
-    <col min="72" max="72" width="26.5546875" style="3" customWidth="1"/>
-    <col min="73" max="73" width="33.33203125" style="3" customWidth="1"/>
-    <col min="74" max="74" width="37.6640625" style="3" customWidth="1"/>
-    <col min="75" max="75" width="35.109375" style="3" customWidth="1"/>
-    <col min="76" max="76" width="36.5546875" style="3" customWidth="1"/>
-    <col min="77" max="77" width="19.88671875" style="3" customWidth="1"/>
-    <col min="78" max="78" width="31.5546875" style="3" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" style="3" customWidth="1"/>
-    <col min="80" max="80" width="21.88671875" style="3" customWidth="1"/>
-    <col min="81" max="81" width="20.6640625" style="3" customWidth="1"/>
-    <col min="82" max="82" width="38.88671875" style="3" customWidth="1"/>
-    <col min="83" max="83" width="25.44140625" style="3" customWidth="1"/>
-    <col min="84" max="84" width="33.5546875" style="3" customWidth="1"/>
-    <col min="85" max="85" width="35.33203125" style="3" customWidth="1"/>
-    <col min="86" max="86" width="35.6640625" style="3" customWidth="1"/>
-    <col min="87" max="87" width="32.33203125" style="3" customWidth="1"/>
-    <col min="88" max="88" width="29.6640625" style="3" customWidth="1"/>
-    <col min="89" max="89" width="19.6640625" style="3" customWidth="1"/>
-    <col min="90" max="90" width="24.44140625" style="3" customWidth="1"/>
-    <col min="91" max="91" width="32.44140625" style="3" customWidth="1"/>
-    <col min="92" max="92" width="36.88671875" style="3" customWidth="1"/>
-    <col min="93" max="93" width="14.5546875" style="3" customWidth="1"/>
-    <col min="94" max="16384" width="9.109375" style="3"/>
+    <col min="65" max="65" width="35.7109375" style="3" customWidth="1"/>
+    <col min="66" max="66" width="39.28515625" style="3" customWidth="1"/>
+    <col min="67" max="67" width="31.42578125" style="3" customWidth="1"/>
+    <col min="68" max="69" width="9.140625" style="3"/>
+    <col min="70" max="70" width="29.42578125" style="3" customWidth="1"/>
+    <col min="71" max="71" width="36.85546875" style="3" customWidth="1"/>
+    <col min="72" max="72" width="26.5703125" style="3" customWidth="1"/>
+    <col min="73" max="73" width="33.28515625" style="3" customWidth="1"/>
+    <col min="74" max="74" width="37.7109375" style="3" customWidth="1"/>
+    <col min="75" max="75" width="35.140625" style="3" customWidth="1"/>
+    <col min="76" max="76" width="36.5703125" style="3" customWidth="1"/>
+    <col min="77" max="77" width="19.85546875" style="3" customWidth="1"/>
+    <col min="78" max="78" width="31.5703125" style="3" customWidth="1"/>
+    <col min="79" max="79" width="19.28515625" style="3" customWidth="1"/>
+    <col min="80" max="80" width="21.85546875" style="3" customWidth="1"/>
+    <col min="81" max="81" width="20.7109375" style="3" customWidth="1"/>
+    <col min="82" max="82" width="38.85546875" style="3" customWidth="1"/>
+    <col min="83" max="83" width="25.42578125" style="3" customWidth="1"/>
+    <col min="84" max="84" width="33.5703125" style="3" customWidth="1"/>
+    <col min="85" max="85" width="35.28515625" style="3" customWidth="1"/>
+    <col min="86" max="86" width="35.7109375" style="3" customWidth="1"/>
+    <col min="87" max="87" width="32.28515625" style="3" customWidth="1"/>
+    <col min="88" max="88" width="29.7109375" style="3" customWidth="1"/>
+    <col min="89" max="89" width="19.7109375" style="3" customWidth="1"/>
+    <col min="90" max="90" width="24.42578125" style="3" customWidth="1"/>
+    <col min="91" max="91" width="32.42578125" style="3" customWidth="1"/>
+    <col min="92" max="92" width="36.85546875" style="3" customWidth="1"/>
+    <col min="93" max="93" width="14.5703125" style="3" customWidth="1"/>
+    <col min="94" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -905,7 +901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -993,7 +989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1030,7 +1026,7 @@
       <c r="T3" s="6"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1063,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1084,22 +1080,22 @@
         <v>38</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="6">
-        <v>4373388</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>67</v>
+      <c r="H5" s="10">
+        <v>4383359</v>
+      </c>
+      <c r="I5" s="10">
+        <v>4383359</v>
+      </c>
+      <c r="J5" s="10">
+        <v>4383359</v>
+      </c>
+      <c r="K5" s="10">
+        <v>4383359</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -1114,9 +1110,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>